<commit_message>
Add CVAudio Settings and ChangeReadedTextColor function
</commit_message>
<xml_diff>
--- a/AVGFrame/Assets/StreamingAssets/chapter.xlsx
+++ b/AVGFrame/Assets/StreamingAssets/chapter.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="146">
   <si>
     <t>Index</t>
   </si>
@@ -105,7 +105,7 @@
     <t>bg7</t>
   </si>
   <si>
-    <t>粉色</t>
+    <t>粉</t>
   </si>
   <si>
     <t>pink0</t>
@@ -120,7 +120,7 @@
     <t>人家和老公亲热着呢，哪有功夫搭理咱们单身狗啊。</t>
   </si>
   <si>
-    <t>橙色</t>
+    <t>橙</t>
   </si>
   <si>
     <t>pink0/orange0</t>
@@ -195,9 +195,6 @@
     <t>真是的，来的太晚了啦！</t>
   </si>
   <si>
-    <t>粉</t>
-  </si>
-  <si>
     <t>man0/pink0</t>
   </si>
   <si>
@@ -361,9 +358,6 @@
   </si>
   <si>
     <t>bg11</t>
-  </si>
-  <si>
-    <t>橙</t>
   </si>
   <si>
     <t>orange0</t>
@@ -482,14 +476,105 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -504,99 +589,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -610,8 +603,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -634,7 +628,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,55 +700,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,31 +724,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,13 +742,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,13 +766,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,7 +778,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,7 +790,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,24 +822,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -857,6 +833,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,11 +874,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -902,26 +911,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -933,145 +927,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1433,7 +1427,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2042,10 +2036,10 @@
         <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>36</v>
@@ -2065,7 +2059,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>49</v>
@@ -2083,7 +2077,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>49</v>
@@ -2112,22 +2106,22 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2138,10 +2132,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2156,10 +2150,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2174,10 +2168,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2192,10 +2186,10 @@
         <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>50</v>
@@ -2207,7 +2201,7 @@
         <v>31</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2218,10 +2212,10 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2236,16 +2230,16 @@
         <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>36</v>
@@ -2262,16 +2256,16 @@
         <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>36</v>
@@ -2288,10 +2282,10 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2306,10 +2300,10 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2324,16 +2318,16 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>52</v>
@@ -2350,10 +2344,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2368,10 +2362,10 @@
         <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>50</v>
@@ -2383,7 +2377,7 @@
         <v>52</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2394,22 +2388,22 @@
         <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2420,10 +2414,10 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2438,10 +2432,10 @@
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2453,13 +2447,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2474,10 +2468,10 @@
         <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2492,10 +2486,10 @@
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2510,10 +2504,10 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2528,10 +2522,10 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2542,13 +2536,13 @@
         <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>30</v>
@@ -2557,7 +2551,7 @@
         <v>52</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -2565,20 +2559,20 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="J34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2586,13 +2580,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2604,13 +2598,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2625,13 +2619,13 @@
         <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>30</v>
@@ -2640,7 +2634,7 @@
         <v>52</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2651,10 +2645,10 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2665,13 +2659,13 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>30</v>
@@ -2680,7 +2674,7 @@
         <v>52</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2691,13 +2685,13 @@
         <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>30</v>
@@ -2706,7 +2700,7 @@
         <v>52</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2717,10 +2711,10 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2731,10 +2725,10 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2745,10 +2739,10 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2756,7 +2750,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2767,22 +2761,22 @@
         <v>26</v>
       </c>
       <c r="C45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" t="s">
         <v>114</v>
       </c>
-      <c r="E45" t="s">
+      <c r="G45" t="s">
         <v>115</v>
       </c>
-      <c r="F45" t="s">
+      <c r="H45" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G45" t="s">
-        <v>117</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2793,10 +2787,10 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -2808,10 +2802,10 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2822,19 +2816,19 @@
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" t="s">
         <v>114</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>115</v>
-      </c>
-      <c r="F48" t="s">
-        <v>116</v>
-      </c>
-      <c r="G48" t="s">
-        <v>117</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>37</v>
@@ -2848,16 +2842,16 @@
         <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E49" t="s">
         <v>50</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>36</v>
@@ -2874,10 +2868,10 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2888,19 +2882,19 @@
         <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D51" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" t="s">
         <v>114</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" t="s">
         <v>115</v>
-      </c>
-      <c r="F51" t="s">
-        <v>116</v>
-      </c>
-      <c r="G51" t="s">
-        <v>117</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>39</v>
@@ -2914,22 +2908,22 @@
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52" t="s">
         <v>50</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2937,17 +2931,17 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G53" s="1"/>
       <c r="J53" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2958,22 +2952,22 @@
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" t="s">
+        <v>34</v>
+      </c>
+      <c r="F54" t="s">
         <v>114</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>115</v>
       </c>
-      <c r="F54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G54" t="s">
-        <v>117</v>
-      </c>
       <c r="H54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2981,16 +2975,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J55" t="s">
         <v>131</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J55" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3001,10 +2995,10 @@
         <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>50</v>
@@ -3016,7 +3010,7 @@
         <v>52</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3027,10 +3021,10 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E57" s="1"/>
     </row>
@@ -3042,10 +3036,10 @@
         <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>50</v>
@@ -3054,10 +3048,10 @@
         <v>51</v>
       </c>
       <c r="G58" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -3068,22 +3062,22 @@
         <v>26</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3094,22 +3088,22 @@
         <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3120,22 +3114,22 @@
         <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3146,10 +3140,10 @@
         <v>26</v>
       </c>
       <c r="C62" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>50</v>
@@ -3161,7 +3155,7 @@
         <v>52</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3172,10 +3166,10 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E63" s="1"/>
     </row>
@@ -3187,22 +3181,22 @@
         <v>26</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -3213,10 +3207,10 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -3227,10 +3221,10 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3238,7 +3232,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>